<commit_message>
Add inheritance template & cfg formating
</commit_message>
<xml_diff>
--- a/input/L2.xlsx
+++ b/input/L2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Device</t>
   </si>
@@ -29,6 +29,9 @@
     <t>10.32.5.5</t>
   </si>
   <si>
+    <t>interface type</t>
+  </si>
+  <si>
     <t>interface</t>
   </si>
   <si>
@@ -39,6 +42,9 @@
   </si>
   <si>
     <t>lab-switch</t>
+  </si>
+  <si>
+    <t>fastethernet</t>
   </si>
   <si>
     <t>0/1</t>
@@ -212,162 +218,201 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
         <v>254.0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
         <v>17.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1">
         <v>17.0</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Auto discover xlsx templates columns
</commit_message>
<xml_diff>
--- a/input/L2.xlsx
+++ b/input/L2.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="IP &amp; Credentials" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Phiscal layout" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="lab-switch" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="6lab-sw1" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,21 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="28">
   <si>
     <t>Device</t>
-  </si>
-  <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Credential</t>
-  </si>
-  <si>
-    <t>lab-gw</t>
-  </si>
-  <si>
-    <t>10.32.5.5</t>
   </si>
   <si>
     <t>interface type</t>
@@ -170,9 +158,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="3" max="3" width="18.43"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -184,14 +169,204 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>254.0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -210,209 +385,197 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>254.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>17.0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1">
         <v>17.0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add Port-Channel Support to L2
</commit_message>
<xml_diff>
--- a/input/L2.xlsx
+++ b/input/L2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>interface type</t>
   </si>
@@ -22,6 +22,15 @@
     <t>vlan</t>
   </si>
   <si>
+    <t>allowed vlans</t>
+  </si>
+  <si>
+    <t>channel-group</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
     <t>description/name</t>
   </si>
   <si>
@@ -76,12 +85,18 @@
     <t>0/8</t>
   </si>
   <si>
+    <t>on</t>
+  </si>
+  <si>
     <t>0/9</t>
   </si>
   <si>
     <t>0/10</t>
   </si>
   <si>
+    <t>active</t>
+  </si>
+  <si>
     <t>0/11</t>
   </si>
   <si>
@@ -98,6 +113,12 @@
   </si>
   <si>
     <t>LAB-INFRA</t>
+  </si>
+  <si>
+    <t>port-channel</t>
+  </si>
+  <si>
+    <t>Agg cisco-GW</t>
   </si>
 </sst>
 </file>
@@ -157,7 +178,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="17.14"/>
+    <col customWidth="1" min="2" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="5.14"/>
+    <col customWidth="1" min="4" max="4" width="11.86"/>
+    <col customWidth="1" min="5" max="5" width="12.57"/>
+    <col customWidth="1" min="6" max="6" width="5.71"/>
+    <col customWidth="1" min="7" max="7" width="15.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -173,149 +199,194 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>254.0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>17.0</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>17.0</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -325,8 +396,8 @@
       <c r="C14" s="1">
         <v>254.0</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
+      <c r="G14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -336,8 +407,8 @@
       <c r="C15" s="1">
         <v>16.0</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>27</v>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16">
@@ -347,13 +418,39 @@
       <c r="C16" s="1">
         <v>17.0</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
+      <c r="G16" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>